<commit_message>
edited test sheets to conform to current formatting protocol
</commit_message>
<xml_diff>
--- a/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph_output-2.xlsx
+++ b/test_files/sixteen_tests/4-genes_6-edges_artificial-data_MM_estimation_fixP-0_graph_output-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="0" windowWidth="25360" windowHeight="15280" tabRatio="644" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="644" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -227,31 +227,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -658,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -670,144 +664,97 @@
     <col min="2" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-    </row>
-    <row r="2" spans="1:7" ht="13">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>0.5</v>
       </c>
-      <c r="G2"/>
-    </row>
-    <row r="3" spans="1:7" ht="13">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="G3"/>
-    </row>
-    <row r="4" spans="1:7" ht="13">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="G4"/>
-    </row>
-    <row r="5" spans="1:7" ht="13">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="G5"/>
-    </row>
-    <row r="6" spans="1:7" ht="13">
-      <c r="A6"/>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="B6" s="2"/>
-      <c r="G6"/>
-    </row>
-    <row r="7" spans="1:7" ht="13">
-      <c r="A7"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" s="2"/>
-      <c r="G7"/>
-    </row>
-    <row r="8" spans="1:7" ht="13">
-      <c r="A8"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" s="2"/>
-      <c r="G8"/>
-    </row>
-    <row r="9" spans="1:7" ht="13">
-      <c r="A9"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" s="2"/>
-      <c r="G9"/>
-    </row>
-    <row r="10" spans="1:7" ht="13">
-      <c r="A10"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="B10" s="2"/>
-      <c r="G10"/>
-    </row>
-    <row r="11" spans="1:7" ht="13">
-      <c r="A11"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="B11" s="2"/>
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:7" ht="13">
-      <c r="A12"/>
+    </row>
+    <row r="12" spans="1:4">
       <c r="B12" s="2"/>
-      <c r="G12"/>
-    </row>
-    <row r="13" spans="1:7" ht="13">
-      <c r="A13"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="B13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:7" ht="13">
-      <c r="A14"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="B14" s="2"/>
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:7" ht="13">
-      <c r="A15"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="B15" s="2"/>
-      <c r="G15"/>
-    </row>
-    <row r="16" spans="1:7" ht="13">
-      <c r="A16"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="B16" s="2"/>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="1:7" ht="13">
-      <c r="A17"/>
+    </row>
+    <row r="17" spans="2:4">
       <c r="B17" s="2"/>
-      <c r="G17"/>
-    </row>
-    <row r="18" spans="1:7" ht="13">
-      <c r="A18"/>
+    </row>
+    <row r="18" spans="2:4">
       <c r="B18" s="2"/>
-      <c r="G18"/>
-    </row>
-    <row r="19" spans="1:7" ht="13">
-      <c r="A19"/>
+    </row>
+    <row r="19" spans="2:4">
       <c r="B19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="G19"/>
-    </row>
-    <row r="20" spans="1:7" ht="13">
-      <c r="A20"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4">
       <c r="B20" s="2"/>
-      <c r="G20"/>
-    </row>
-    <row r="21" spans="1:7" ht="13">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="1:7" ht="13">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="G22"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="D24" s="3"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="D24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -827,7 +774,7 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1190,7 +1137,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1298,7 +1245,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1406,14 +1353,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1"/>
-    <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1471,7 +1416,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1578,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1702,7 +1647,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1732,7 +1677,7 @@
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1740,7 +1685,7 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1748,48 +1693,48 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="B6" s="3"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="B7" s="3"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="B8" s="3"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="B9" s="3"/>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="B10" s="3"/>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2">
-      <c r="B11" s="3"/>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="B12" s="3"/>
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2">
-      <c r="B13" s="3"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="B14" s="3"/>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="B15" s="3"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="B16" s="3"/>
+      <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="3"/>
+      <c r="B17" s="2"/>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="3"/>
+      <c r="B18" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1809,7 +1754,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1857,7 +1802,7 @@
       <c r="M1" s="6">
         <v>1.6</v>
       </c>
-      <c r="N1" s="4"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
@@ -2024,32 +1969,32 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="F6" s="5"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="I10" s="5"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="F12" s="5"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="H14" s="5"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="B16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="B16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="18" spans="3:12">
-      <c r="H18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="H18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" spans="3:12">
-      <c r="C19" s="5"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="3:12">
-      <c r="E20" s="5"/>
-      <c r="L20" s="5"/>
+      <c r="E20" s="3"/>
+      <c r="L20" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2069,7 +2014,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="A1:XFD1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2117,7 +2062,7 @@
       <c r="M1" s="6">
         <v>1.6</v>
       </c>
-      <c r="N1" s="4"/>
+      <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
@@ -2284,52 +2229,52 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="B6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="B6" s="3"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="K7" s="5"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="E9" s="5"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="E11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="E11" s="3"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="H12" s="5"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="E13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="E13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="F14" s="5"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="B15" s="5"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="18" spans="6:13">
-      <c r="F18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="F18" s="3"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" spans="6:13">
-      <c r="H19" s="5"/>
-      <c r="L19" s="5"/>
+      <c r="H19" s="3"/>
+      <c r="L19" s="3"/>
     </row>
     <row r="20" spans="6:13">
-      <c r="H20" s="5"/>
-      <c r="K20" s="5"/>
+      <c r="H20" s="3"/>
+      <c r="K20" s="3"/>
     </row>
     <row r="22" spans="6:13">
-      <c r="K22" s="5"/>
-      <c r="M22" s="5"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2347,114 +2292,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="11" style="3"/>
+    <col min="1" max="1" width="5.7109375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2475,34 +2418,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="5.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="5.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2539,16 +2480,16 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2556,16 +2497,16 @@
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2573,16 +2514,16 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2590,16 +2531,16 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2620,8 +2561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2642,7 +2583,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>1E-3</v>
       </c>
     </row>
@@ -2658,7 +2599,7 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>1000000</v>
       </c>
     </row>
@@ -2666,7 +2607,7 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
@@ -2674,7 +2615,7 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>1000000</v>
       </c>
     </row>
@@ -2682,7 +2623,7 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
@@ -2690,7 +2631,7 @@
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2698,7 +2639,7 @@
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2706,7 +2647,7 @@
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="4">
         <v>1</v>
       </c>
     </row>
@@ -2714,7 +2655,7 @@
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="4">
         <v>1</v>
       </c>
     </row>
@@ -2722,7 +2663,7 @@
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2730,7 +2671,7 @@
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="4">
         <v>0</v>
       </c>
     </row>
@@ -2738,7 +2679,7 @@
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="4">
         <v>0.4</v>
       </c>
       <c r="C14" s="1">
@@ -2848,7 +2789,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2897,10 +2838,10 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="5"/>
+      <c r="A11" s="3"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="5"/>
+      <c r="A17" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2918,7 +2859,7 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>